<commit_message>
added most input files
</commit_message>
<xml_diff>
--- a/ontologies/molecular_graph/experiments/most_graph_experiments.xlsx
+++ b/ontologies/molecular_graph/experiments/most_graph_experiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/molecular_graph/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/molecular_graph/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB36C70-D63F-3A47-82E6-B846328A748C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9FB341-E1DF-D040-8EE8-28644B364C40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,15 @@
     <sheet name="nonisolated_loopless2most_graph" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_graph2nonisolated_loopless!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nonisolated_loopless2most_graph!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_graph2nonisolated_loopless!$A$1:$L$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nonisolated_loopless2most_graph!$A$1:$L$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -242,7 +242,55 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -625,10 +673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,10 +694,11 @@
     <col min="10" max="10" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="33.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -685,11 +735,11 @@
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>43390</v>
       </c>
@@ -729,12 +779,16 @@
       <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="8" t="str">
+      <c r="M2" s="1" t="str">
+        <f>L2&amp;" %"&amp;C2</f>
+        <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %1</v>
+      </c>
+      <c r="N2" s="8" t="str">
         <f>"\lstinputlisting[style=p9proof,label="&amp;D2&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C2&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D2&amp;".proof}"</f>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_1,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#1 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_1.proof}</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>43390</v>
       </c>
@@ -774,12 +828,16 @@
       <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="8" t="str">
-        <f t="shared" ref="M3:M10" si="3">"\lstinputlisting[style=p9proof,label="&amp;D3&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C3&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D3&amp;".proof}"</f>
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M10" si="3">L3&amp;" %"&amp;C3</f>
+        <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %2</v>
+      </c>
+      <c r="N3" s="8" t="str">
+        <f t="shared" ref="N3:N10" si="4">"\lstinputlisting[style=p9proof,label="&amp;D3&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C3&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D3&amp;".proof}"</f>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_2,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#2 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_2.proof}</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>43390</v>
       </c>
@@ -819,12 +877,16 @@
       <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="8" t="str">
+      <c r="M4" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all l (line(l) -&gt; (exists x exists y (point(x) &amp; point(y) &amp; x != y &amp; in(x,l) &amp; in(y,l))))). %3</v>
+      </c>
+      <c r="N4" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_3,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#3 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_3.proof}</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>43390</v>
       </c>
@@ -864,12 +926,16 @@
       <c r="L5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="8" t="str">
+      <c r="M5" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %4</v>
+      </c>
+      <c r="N5" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_4,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#4 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_4.proof}</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>43390</v>
       </c>
@@ -909,12 +975,16 @@
       <c r="L6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="8" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x (point(x) | line(x) -&gt; in(x,x))). %5</v>
+      </c>
+      <c r="N6" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_5,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#5 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_5.proof}</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>43390</v>
       </c>
@@ -954,12 +1024,16 @@
       <c r="L7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="8" t="str">
+      <c r="M7" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all p (point(p) -&gt; -line(p))). %6</v>
+      </c>
+      <c r="N7" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_6,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#6 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_6.proof}</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>43390</v>
       </c>
@@ -999,12 +1073,16 @@
       <c r="L8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="8" t="str">
+      <c r="M8" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %7</v>
+      </c>
+      <c r="N8" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_7,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#7 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_7.proof}</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>43390</v>
       </c>
@@ -1044,12 +1122,16 @@
       <c r="L9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="8" t="str">
+      <c r="M9" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %8</v>
+      </c>
+      <c r="N9" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_8,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#8 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_8.proof}</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>43390</v>
       </c>
@@ -1089,20 +1171,481 @@
       <c r="L10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="8" t="str">
+      <c r="M10" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all p (point(p) -&gt; (exists l (line(l) &amp; in(p,l))))). %9</v>
+      </c>
+      <c r="N10" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_9,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#9 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_9.proof}</v>
       </c>
     </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>TEXT(A11,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>I11&amp;"2"&amp;J11&amp;"_"&amp;C11</f>
+        <v>most_graph2nonisolated_loopless_1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3">
+        <v>60</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3">
+        <v>60</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f>I11&amp;"2"&amp;J11</f>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f>L11&amp;" %"&amp;C11</f>
+        <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %1</v>
+      </c>
+      <c r="N11" s="8" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D11&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C11&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D11&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_1,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#1 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_1.proof}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f t="shared" ref="B12:B19" si="5">TEXT(A12,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" ref="D12:D19" si="6">I12&amp;"2"&amp;J12&amp;"_"&amp;C12</f>
+        <v>most_graph2nonisolated_loopless_2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3">
+        <v>60</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="3">
+        <v>60</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" ref="K12:K19" si="7">I12&amp;"2"&amp;J12</f>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f t="shared" ref="M12:M19" si="8">L12&amp;" %"&amp;C12</f>
+        <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %2</v>
+      </c>
+      <c r="N12" s="8" t="str">
+        <f t="shared" ref="N12:N19" si="9">"\lstinputlisting[style=p9proof,label="&amp;D12&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C12&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D12&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_2,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#2 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_2.proof}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3">
+        <v>60</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="3">
+        <v>60</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all l (line(l) -&gt; (exists x exists y (point(x) &amp; point(y) &amp; x != y &amp; in(x,l) &amp; in(y,l))))). %3</v>
+      </c>
+      <c r="N13" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_3,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#3 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_3.proof}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3">
+        <v>60</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %4</v>
+      </c>
+      <c r="N14" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_4,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#4 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_4.proof}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3">
+        <v>60</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x (point(x) | line(x) -&gt; in(x,x))). %5</v>
+      </c>
+      <c r="N15" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_5,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#5 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_5.proof}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3">
+        <v>60</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all p (point(p) -&gt; -line(p))). %6</v>
+      </c>
+      <c r="N16" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_6,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#6 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_6.proof}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="3">
+        <v>60</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="3">
+        <v>60</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %7</v>
+      </c>
+      <c r="N17" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_7,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#7 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_7.proof}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3">
+        <v>60</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="3">
+        <v>60</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %8</v>
+      </c>
+      <c r="N18" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_8,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#8 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_8.proof}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>most_graph2nonisolated_loopless_9</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="3">
+        <v>60</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="3">
+        <v>60</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all p (point(p) -&gt; (exists l (line(l) &amp; in(p,l))))). %9</v>
+      </c>
+      <c r="N19" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_9,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#9 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_9.proof}</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L19" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <dateGroupItem year="2018" month="10" day="19" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G10">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E19">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G19">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1113,10 +1656,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996D9C58-6018-1D42-9792-6063C3F60A8A}">
-  <dimension ref="A1:M10"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1133,10 +1677,11 @@
     <col min="10" max="10" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="79.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1173,11 +1718,11 @@
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>43390</v>
       </c>
@@ -1217,12 +1762,16 @@
       <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="8" t="str">
+      <c r="M2" s="1" t="str">
+        <f>L2&amp;" %"&amp;C2</f>
+        <v>(all x mol(x,x)). %1</v>
+      </c>
+      <c r="N2" s="8" t="str">
         <f>"\lstinputlisting[style=p9proof,label="&amp;D2&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C2&amp;" in $T_{most\_graph}$]{proofs/"&amp;D2&amp;".proof}"</f>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_1,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#1 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_1.proof}</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>43390</v>
       </c>
@@ -1262,12 +1811,16 @@
       <c r="L3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="8" t="str">
-        <f t="shared" ref="M3:M10" si="3">"\lstinputlisting[style=p9proof,label="&amp;D3&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C3&amp;" in $T_{most\_graph}$]{proofs/"&amp;D3&amp;".proof}"</f>
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M10" si="3">L3&amp;" %"&amp;C3</f>
+        <v>(all x all y (mol(x,y) -&gt; mol(y,x))). %2</v>
+      </c>
+      <c r="N3" s="8" t="str">
+        <f t="shared" ref="N3:N10" si="4">"\lstinputlisting[style=p9proof,label="&amp;D3&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C3&amp;" in $T_{most\_graph}$]{proofs/"&amp;D3&amp;".proof}"</f>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_2,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#2 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_2.proof}</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>43390</v>
       </c>
@@ -1307,12 +1860,16 @@
       <c r="L4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="8" t="str">
+      <c r="M4" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x all y (mol(x,y) &amp; atom(x) &amp; atom(y) -&gt; x = y)). %3</v>
+      </c>
+      <c r="N4" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_3,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#3 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_3.proof}</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>43390</v>
       </c>
@@ -1352,12 +1909,16 @@
       <c r="L5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="8" t="str">
+      <c r="M5" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x all y (mol(x,y) &amp; bond(x) &amp; bond(y) -&gt; x = y)). %4</v>
+      </c>
+      <c r="N5" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_4,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#4 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_4.proof}</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>43390</v>
       </c>
@@ -1397,12 +1958,16 @@
       <c r="L6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="8" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x all y all z all b (atom(x) &amp; atom(y) &amp; atom(z) &amp; bond(b) &amp; mol(x,b) &amp; mol(y,b) &amp; mol(z,b) -&gt; x = y | x = z | y = z)). %5</v>
+      </c>
+      <c r="N6" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_5,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#5 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_5.proof}</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>43390</v>
       </c>
@@ -1442,12 +2007,16 @@
       <c r="L7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="8" t="str">
+      <c r="M7" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all x (atom(x) -&gt; (exists b exists y (atom(y) &amp; bond(b) &amp; mol(x,b) &amp; mol(y,b))))). %6</v>
+      </c>
+      <c r="N7" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_6,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#6 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_6.proof}</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>43390</v>
       </c>
@@ -1487,12 +2056,16 @@
       <c r="L8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="8" t="str">
+      <c r="M8" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y (atom(x) &amp; atom(y) &amp; mol(x,b) &amp; mol(y,b))))). %7</v>
+      </c>
+      <c r="N8" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_7,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#7 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_7.proof}</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>43390</v>
       </c>
@@ -1532,12 +2105,16 @@
       <c r="L9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="8" t="str">
+      <c r="M9" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y all z1 all z2 (atom(x) &amp; atom(y) &amp; atom(z1) &amp; atom(z2) &amp; mol(z1,b) &amp; mol(z2,b) -&gt; z1 = x | z1 = y | z2 = x | z2 = y)))). %8</v>
+      </c>
+      <c r="N9" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_8,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#8 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_8.proof}</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>43390</v>
       </c>
@@ -1577,19 +2154,480 @@
       <c r="L10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="8" t="str">
+      <c r="M10" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y (atom(x) &amp; atom(y) &amp; mol(x,b) &amp; mol(y,b) &amp; y != x)))). %9</v>
+      </c>
+      <c r="N10" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_9,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#9 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_9.proof}</v>
       </c>
     </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>TEXT(A11,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>I11&amp;"2"&amp;J11&amp;"_"&amp;C11</f>
+        <v>nonisolated_loopless2most_graph_1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3">
+        <v>60</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3">
+        <v>60</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f>I11&amp;"2"&amp;J11</f>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f>L11&amp;" %"&amp;C11</f>
+        <v>(all x mol(x,x)). %1</v>
+      </c>
+      <c r="N11" s="8" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D11&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C11&amp;" in $T_{most\_graph}$]{proofs/"&amp;D11&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_1,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#1 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_1.proof}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f t="shared" ref="B12:B19" si="5">TEXT(A12,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" ref="D12:D19" si="6">I12&amp;"2"&amp;J12&amp;"_"&amp;C12</f>
+        <v>nonisolated_loopless2most_graph_2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3">
+        <v>60</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="3">
+        <v>60</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" ref="K12:K19" si="7">I12&amp;"2"&amp;J12</f>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f t="shared" ref="M12:M19" si="8">L12&amp;" %"&amp;C12</f>
+        <v>(all x all y (mol(x,y) -&gt; mol(y,x))). %2</v>
+      </c>
+      <c r="N12" s="8" t="str">
+        <f t="shared" ref="N12:N19" si="9">"\lstinputlisting[style=p9proof,label="&amp;D12&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C12&amp;" in $T_{most\_graph}$]{proofs/"&amp;D12&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_2,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#2 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_2.proof}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3">
+        <v>60</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="3">
+        <v>60</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x all y (mol(x,y) &amp; atom(x) &amp; atom(y) -&gt; x = y)). %3</v>
+      </c>
+      <c r="N13" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_3,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#3 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_3.proof}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3">
+        <v>60</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x all y (mol(x,y) &amp; bond(x) &amp; bond(y) -&gt; x = y)). %4</v>
+      </c>
+      <c r="N14" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_4,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#4 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_4.proof}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3">
+        <v>60</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x all y all z all b (atom(x) &amp; atom(y) &amp; atom(z) &amp; bond(b) &amp; mol(x,b) &amp; mol(y,b) &amp; mol(z,b) -&gt; x = y | x = z | y = z)). %5</v>
+      </c>
+      <c r="N15" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_5,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#5 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_5.proof}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3">
+        <v>60</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all x (atom(x) -&gt; (exists b exists y (atom(y) &amp; bond(b) &amp; mol(x,b) &amp; mol(y,b))))). %6</v>
+      </c>
+      <c r="N16" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_6,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#6 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_6.proof}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="3">
+        <v>60</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="3">
+        <v>60</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y (atom(x) &amp; atom(y) &amp; mol(x,b) &amp; mol(y,b))))). %7</v>
+      </c>
+      <c r="N17" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_7,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#7 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_7.proof}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3">
+        <v>60</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="3">
+        <v>60</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y all z1 all z2 (atom(x) &amp; atom(y) &amp; atom(z1) &amp; atom(z2) &amp; mol(z1,b) &amp; mol(z2,b) -&gt; z1 = x | z1 = y | z2 = x | z2 = y)))). %8</v>
+      </c>
+      <c r="N18" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_8,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#8 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_8.proof}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>43392</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1019_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>nonisolated_loopless2most_graph_9</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="3">
+        <v>60</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="3">
+        <v>60</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y (atom(x) &amp; atom(y) &amp; mol(x,b) &amp; mol(y,b) &amp; y != x)))). %9</v>
+      </c>
+      <c r="N19" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_9,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#9 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_9.proof}</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L19" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <dateGroupItem year="2018" month="10" day="19" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="E2:E10">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E19">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G11:G19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>

<commit_message>
uploaded updated most_graph experiments spreadsheet
</commit_message>
<xml_diff>
--- a/ontologies/molecular_graph/experiments/most_graph_experiments.xlsx
+++ b/ontologies/molecular_graph/experiments/most_graph_experiments.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/molecular_graph/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9FB341-E1DF-D040-8EE8-28644B364C40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2985A2-9074-8449-9119-5F76E003CF64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="most_graph2nonisolated_loopless" sheetId="1" r:id="rId1"/>
     <sheet name="nonisolated_loopless2most_graph" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_graph2nonisolated_loopless!$A$1:$L$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nonisolated_loopless2most_graph!$A$1:$L$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_graph2nonisolated_loopless!$A$1:$L$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nonisolated_loopless2most_graph!$A$1:$L$28</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -242,7 +242,55 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -674,10 +722,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -693,7 +741,7 @@
     <col min="9" max="9" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="79.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37" style="1" customWidth="1"/>
     <col min="13" max="13" width="33.83203125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
@@ -1180,7 +1228,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_9,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#9 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_9.proof}</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>43392</v>
       </c>
@@ -1229,7 +1277,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_1,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#1 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_1.proof}</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>43392</v>
       </c>
@@ -1278,7 +1326,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_2,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#2 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_2.proof}</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>43392</v>
       </c>
@@ -1327,7 +1375,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_3,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#3 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_3.proof}</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>43392</v>
       </c>
@@ -1376,7 +1424,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_4,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#4 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_4.proof}</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>43392</v>
       </c>
@@ -1425,7 +1473,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_5,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#5 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_5.proof}</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>43392</v>
       </c>
@@ -1474,7 +1522,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_6,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#6 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_6.proof}</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>43392</v>
       </c>
@@ -1523,7 +1571,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_7,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#7 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_7.proof}</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>43392</v>
       </c>
@@ -1572,7 +1620,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_8,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#8 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_8.proof}</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>43392</v>
       </c>
@@ -1621,31 +1669,482 @@
         <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_9,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#9 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_9.proof}</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>TEXT(A20,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>I20&amp;"2"&amp;J20&amp;"_"&amp;C20</f>
+        <v>most_graph2nonisolated_loopless_1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3">
+        <v>60</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="3">
+        <v>60</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f>I20&amp;"2"&amp;J20</f>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="1" t="str">
+        <f>L20&amp;" %"&amp;C20</f>
+        <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %1</v>
+      </c>
+      <c r="N20" s="8" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D20&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C20&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D20&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_1,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#1 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_1.proof}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" ref="B21:B28" si="10">TEXT(A21,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" ref="D21:D28" si="11">I21&amp;"2"&amp;J21&amp;"_"&amp;C21</f>
+        <v>most_graph2nonisolated_loopless_2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3">
+        <v>60</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="3">
+        <v>60</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" ref="K21:K28" si="12">I21&amp;"2"&amp;J21</f>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="1" t="str">
+        <f t="shared" ref="M21:M28" si="13">L21&amp;" %"&amp;C21</f>
+        <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %2</v>
+      </c>
+      <c r="N21" s="8" t="str">
+        <f t="shared" ref="N21:N28" si="14">"\lstinputlisting[style=p9proof,label="&amp;D21&amp;",caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#"&amp;C21&amp;" in $T_{nonisolated\_loopless}$]{proofs/"&amp;D21&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_2,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#2 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_2.proof}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3">
+        <v>60</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="3">
+        <v>60</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all l (line(l) -&gt; (exists x exists y (point(x) &amp; point(y) &amp; x != y &amp; in(x,l) &amp; in(y,l))))). %3</v>
+      </c>
+      <c r="N22" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_3,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#3 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_3.proof}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="3">
+        <v>60</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="3">
+        <v>60</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %4</v>
+      </c>
+      <c r="N23" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_4,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#4 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_4.proof}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="3">
+        <v>60</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="3">
+        <v>60</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x (point(x) | line(x) -&gt; in(x,x))). %5</v>
+      </c>
+      <c r="N24" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_5,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#5 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_5.proof}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_6</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="3">
+        <v>60</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="3">
+        <v>60</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all p (point(p) -&gt; -line(p))). %6</v>
+      </c>
+      <c r="N25" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_6,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#6 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_6.proof}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="3">
+        <v>60</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="3">
+        <v>60</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %7</v>
+      </c>
+      <c r="N26" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_7,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#7 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_7.proof}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C27" s="1">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_8</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3">
+        <v>60</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="3">
+        <v>60</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %8</v>
+      </c>
+      <c r="N27" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_8,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#8 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_8.proof}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C28" s="1">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>most_graph2nonisolated_loopless_9</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="3">
+        <v>60</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="3">
+        <v>60</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all p (point(p) -&gt; (exists l (line(l) &amp; in(p,l))))). %9</v>
+      </c>
+      <c r="N28" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=most_graph2nonisolated_loopless_9,caption=$T_{most\_graph} \cup \Delta_1 \models$ Axiom \#9 in $T_{nonisolated\_loopless}$]{proofs/most_graph2nonisolated_loopless_9.proof}</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L19" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L28" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="19" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="10" day="20" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G10">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E19">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G19">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E28">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:G28">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1657,10 +2156,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996D9C58-6018-1D42-9792-6063C3F60A8A}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1676,7 +2175,7 @@
     <col min="9" max="9" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="79.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="79.83203125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
@@ -2163,7 +2662,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_9,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#9 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_9.proof}</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>43392</v>
       </c>
@@ -2212,7 +2711,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_1,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#1 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_1.proof}</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>43392</v>
       </c>
@@ -2261,7 +2760,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_2,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#2 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_2.proof}</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>43392</v>
       </c>
@@ -2310,7 +2809,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_3,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#3 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_3.proof}</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>43392</v>
       </c>
@@ -2359,7 +2858,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_4,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#4 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_4.proof}</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>43392</v>
       </c>
@@ -2408,7 +2907,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_5,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#5 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_5.proof}</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>43392</v>
       </c>
@@ -2457,7 +2956,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_6,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#6 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_6.proof}</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>43392</v>
       </c>
@@ -2506,7 +3005,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_7,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#7 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_7.proof}</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>43392</v>
       </c>
@@ -2555,7 +3054,7 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_8,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#8 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_8.proof}</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>43392</v>
       </c>
@@ -2604,30 +3103,481 @@
         <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_9,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#9 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_9.proof}</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>TEXT(A20,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>I20&amp;"2"&amp;J20&amp;"_"&amp;C20</f>
+        <v>nonisolated_loopless2most_graph_1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3">
+        <v>60</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="3">
+        <v>60</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f>I20&amp;"2"&amp;J20</f>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="1" t="str">
+        <f>L20&amp;" %"&amp;C20</f>
+        <v>(all x mol(x,x)). %1</v>
+      </c>
+      <c r="N20" s="8" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D20&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C20&amp;" in $T_{most\_graph}$]{proofs/"&amp;D20&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_1,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#1 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_1.proof}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" ref="B21:B28" si="10">TEXT(A21,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" ref="D21:D28" si="11">I21&amp;"2"&amp;J21&amp;"_"&amp;C21</f>
+        <v>nonisolated_loopless2most_graph_2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3">
+        <v>60</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="3">
+        <v>60</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" ref="K21:K28" si="12">I21&amp;"2"&amp;J21</f>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="1" t="str">
+        <f t="shared" ref="M21:M28" si="13">L21&amp;" %"&amp;C21</f>
+        <v>(all x all y (mol(x,y) -&gt; mol(y,x))). %2</v>
+      </c>
+      <c r="N21" s="8" t="str">
+        <f t="shared" ref="N21:N28" si="14">"\lstinputlisting[style=p9proof,label="&amp;D21&amp;",caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#"&amp;C21&amp;" in $T_{most\_graph}$]{proofs/"&amp;D21&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_2,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#2 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_2.proof}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3">
+        <v>60</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="3">
+        <v>60</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x all y (mol(x,y) &amp; atom(x) &amp; atom(y) -&gt; x = y)). %3</v>
+      </c>
+      <c r="N22" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_3,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#3 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_3.proof}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="3">
+        <v>60</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="3">
+        <v>60</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x all y (mol(x,y) &amp; bond(x) &amp; bond(y) -&gt; x = y)). %4</v>
+      </c>
+      <c r="N23" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_4,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#4 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_4.proof}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="3">
+        <v>60</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="3">
+        <v>60</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x all y all z all b (atom(x) &amp; atom(y) &amp; atom(z) &amp; bond(b) &amp; mol(x,b) &amp; mol(y,b) &amp; mol(z,b) -&gt; x = y | x = z | y = z)). %5</v>
+      </c>
+      <c r="N24" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_5,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#5 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_5.proof}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_6</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="3">
+        <v>60</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="3">
+        <v>60</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all x (atom(x) -&gt; (exists b exists y (atom(y) &amp; bond(b) &amp; mol(x,b) &amp; mol(y,b))))). %6</v>
+      </c>
+      <c r="N25" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_6,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#6 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_6.proof}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="3">
+        <v>60</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="3">
+        <v>60</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y (atom(x) &amp; atom(y) &amp; mol(x,b) &amp; mol(y,b))))). %7</v>
+      </c>
+      <c r="N26" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_7,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#7 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_7.proof}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C27" s="1">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_8</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3">
+        <v>60</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="3">
+        <v>60</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y all z1 all z2 (atom(x) &amp; atom(y) &amp; atom(z1) &amp; atom(z2) &amp; mol(z1,b) &amp; mol(z2,b) -&gt; z1 = x | z1 = y | z2 = x | z2 = y)))). %8</v>
+      </c>
+      <c r="N27" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_8,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#8 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_8.proof}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>43393</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1020_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C28" s="1">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>nonisolated_loopless2most_graph_9</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="3">
+        <v>60</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="3">
+        <v>60</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>nonisolated_loopless2most_graph</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>(all b (bond(b) -&gt; (exists x exists y (atom(x) &amp; atom(y) &amp; mol(x,b) &amp; mol(y,b) &amp; y != x)))). %9</v>
+      </c>
+      <c r="N28" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>\lstinputlisting[style=p9proof,label=nonisolated_loopless2most_graph_9,caption=$T_{nonisolated\_loopless} \cup \Pi_1 \models$ Axiom \#9 in $T_{most\_graph}$]{proofs/nonisolated_loopless2most_graph_9.proof}</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L19" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L28" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="19" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="10" day="20" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E19">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G19">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E28">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G19">
+  <conditionalFormatting sqref="G20:G28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated most experiment spreadsheets
</commit_message>
<xml_diff>
--- a/ontologies/molecular_graph/experiments/most_graph_experiments.xlsx
+++ b/ontologies/molecular_graph/experiments/most_graph_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/molecular_graph/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2985A2-9074-8449-9119-5F76E003CF64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F3BA05-6444-6C4F-A9BE-A35AE982E262}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="most_graph2nonisolated_loopless" sheetId="1" r:id="rId1"/>
@@ -724,7 +724,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M20" sqref="M20:M28"/>
     </sheetView>
   </sheetViews>
@@ -2139,12 +2139,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E28">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G28">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2158,8 +2158,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3553,22 +3553,22 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G10">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E19">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G19">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>